<commit_message>
9.5 questoes para fazer
</commit_message>
<xml_diff>
--- a/abordagem_estatistica/controle_e_exibilidade.xlsx
+++ b/abordagem_estatistica/controle_e_exibilidade.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GuilhermeRed\Documents\Materiais\data_science\abordagem_estatistica\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gbueno\Projects\Git\data_science\abordagem_estatistica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9BB8F1-9E08-4B24-A801-7CE6164B6719}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="10440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="10440"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="3" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -325,43 +324,6 @@
   <si>
     <r>
       <t xml:space="preserve">ESTIMATIVA 2019 PARA O PRODUTO </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>B</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">ESTIMATIVA 2019 PARA O PRODUTO </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>A</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="16"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> E </t>
     </r>
     <r>
       <rPr>
@@ -751,19 +713,22 @@
       <t>)</t>
     </r>
   </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="7">
-    <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="0.00000%"/>
-    <numFmt numFmtId="165" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-[$€-2]\ * #,##0.00000_-;\-[$€-2]\ * #,##0.00000_-;_-[$€-2]\ * &quot;-&quot;?????_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-[$€-2]\ * #,##0.00000_-;\-[$€-2]\ * #,##0.00000_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="169" formatCode="_-[$R$-416]\ * #,##0.00000_-;\-[$R$-416]\ * #,##0.00000_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-&quot;R$&quot;* #,##0.00_-;\-&quot;R$&quot;* #,##0.00_-;_-&quot;R$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="0.00000%"/>
+    <numFmt numFmtId="166" formatCode="_-[$€-2]\ * #,##0.00_-;\-[$€-2]\ * #,##0.00_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-[$€-2]\ * #,##0.00000_-;\-[$€-2]\ * #,##0.00000_-;_-[$€-2]\ * &quot;-&quot;?????_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-[$€-2]\ * #,##0.00000_-;\-[$€-2]\ * #,##0.00000_-;_-[$€-2]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="170" formatCode="_-[$R$-416]\ * #,##0.00000_-;\-[$R$-416]\ * #,##0.00000_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -852,7 +817,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="50">
+  <borders count="53">
     <border>
       <left/>
       <right/>
@@ -1523,13 +1488,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="0"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1544,7 +1548,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1553,13 +1557,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -1567,7 +1571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1583,18 +1587,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -1607,14 +1608,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
@@ -1636,44 +1637,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
@@ -1691,12 +1686,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="41" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1705,25 +1700,25 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1739,22 +1734,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1763,19 +1758,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1800,25 +1816,37 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="51" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1841,7 +1869,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -1880,6 +1908,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1969,7 +1998,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000C-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2016,7 +2045,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2063,7 +2092,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2111,7 +2140,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000002-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2158,7 +2187,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2205,7 +2234,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000A-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2255,7 +2284,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2305,7 +2334,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2355,7 +2384,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000008-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2405,7 +2434,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000006-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2455,7 +2484,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2505,7 +2534,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-0955-452D-9773-D388DC6EFD84}"/>
               </c:ext>
@@ -2515,111 +2544,111 @@
             <c:dLbl>
               <c:idx val="0"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000C-0955-452D-9773-D388DC6EFD84}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-0955-452D-9773-D388DC6EFD84}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-0955-452D-9773-D388DC6EFD84}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-0955-452D-9773-D388DC6EFD84}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000A-0955-452D-9773-D388DC6EFD84}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-0955-452D-9773-D388DC6EFD84}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000007-0955-452D-9773-D388DC6EFD84}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-0955-452D-9773-D388DC6EFD84}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000006-0955-452D-9773-D388DC6EFD84}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-0955-452D-9773-D388DC6EFD84}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000004-0955-452D-9773-D388DC6EFD84}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -2672,8 +2701,10 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:val>
@@ -2721,7 +2752,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-0955-452D-9773-D388DC6EFD84}"/>
             </c:ext>
@@ -2748,6 +2779,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2779,14 +2811,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2822,7 +2854,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -2861,6 +2893,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2950,7 +2983,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -2997,7 +3030,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -3044,7 +3077,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -3092,7 +3125,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -3139,7 +3172,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -3186,7 +3219,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -3236,7 +3269,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000D-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -3286,7 +3319,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000F-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -3336,7 +3369,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000011-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -3386,7 +3419,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000013-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -3436,7 +3469,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000015-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -3486,7 +3519,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000017-0174-4C32-990C-6234D67F333C}"/>
               </c:ext>
@@ -3496,111 +3529,111 @@
             <c:dLbl>
               <c:idx val="0"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-0174-4C32-990C-6234D67F333C}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-0174-4C32-990C-6234D67F333C}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-0174-4C32-990C-6234D67F333C}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-0174-4C32-990C-6234D67F333C}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-0174-4C32-990C-6234D67F333C}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000D-0174-4C32-990C-6234D67F333C}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000F-0174-4C32-990C-6234D67F333C}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000011-0174-4C32-990C-6234D67F333C}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000013-0174-4C32-990C-6234D67F333C}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000015-0174-4C32-990C-6234D67F333C}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000017-0174-4C32-990C-6234D67F333C}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -3653,8 +3686,10 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:val>
@@ -3702,7 +3737,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000018-0174-4C32-990C-6234D67F333C}"/>
             </c:ext>
@@ -3729,6 +3764,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3760,14 +3796,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3803,7 +3839,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="pt-BR"/>
   <c:roundedCorners val="0"/>
@@ -3847,6 +3883,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3936,7 +3973,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -3983,7 +4020,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -4030,7 +4067,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -4039,7 +4076,7 @@
           <c:dPt>
             <c:idx val="3"/>
             <c:bubble3D val="0"/>
-            <c:explosion val="35"/>
+            <c:explosion val="20"/>
             <c:spPr>
               <a:gradFill rotWithShape="1">
                 <a:gsLst>
@@ -4078,7 +4115,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -4125,7 +4162,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -4172,7 +4209,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -4222,7 +4259,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000D-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -4272,7 +4309,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000F-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -4322,7 +4359,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000011-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -4372,7 +4409,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000013-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -4422,7 +4459,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000015-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -4472,7 +4509,7 @@
                 </a:outerShdw>
               </a:effectLst>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000017-C4A6-45F0-AA22-D49C157EE0F3}"/>
               </c:ext>
@@ -4482,111 +4519,111 @@
             <c:dLbl>
               <c:idx val="0"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000001-C4A6-45F0-AA22-D49C157EE0F3}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="1"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-C4A6-45F0-AA22-D49C157EE0F3}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="2"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000005-C4A6-45F0-AA22-D49C157EE0F3}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="4"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000009-C4A6-45F0-AA22-D49C157EE0F3}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="5"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000B-C4A6-45F0-AA22-D49C157EE0F3}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="6"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000D-C4A6-45F0-AA22-D49C157EE0F3}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="7"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000F-C4A6-45F0-AA22-D49C157EE0F3}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="8"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000011-C4A6-45F0-AA22-D49C157EE0F3}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="9"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000013-C4A6-45F0-AA22-D49C157EE0F3}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="10"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000015-C4A6-45F0-AA22-D49C157EE0F3}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:dLbl>
               <c:idx val="11"/>
               <c:delete val="1"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+              <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000017-C4A6-45F0-AA22-D49C157EE0F3}"/>
                 </c:ext>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
               </c:extLst>
             </c:dLbl>
             <c:spPr>
@@ -4639,8 +4676,10 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+              </c:ext>
             </c:extLst>
           </c:dLbls>
           <c:val>
@@ -4688,7 +4727,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000018-C4A6-45F0-AA22-D49C157EE0F3}"/>
             </c:ext>
@@ -4715,6 +4754,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4746,14 +4786,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:extLst>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -6431,7 +6471,7 @@
             <xdr:cNvPr id="2" name="CaixaDeTexto 1">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92405025-90F6-4C07-A384-17EEE1495ADB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{92405025-90F6-4C07-A384-17EEE1495ADB}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -6953,7 +6993,7 @@
             <xdr:cNvPr id="4" name="CaixaDeTexto 3">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B3D3A47-CA75-4DC6-9105-52815B8AC4D4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{2B3D3A47-CA75-4DC6-9105-52815B8AC4D4}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7468,7 +7508,7 @@
             <xdr:cNvPr id="5" name="CaixaDeTexto 4">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5920DD7E-3FBA-4DE1-AD54-97B5A7CF9E2A}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{5920DD7E-3FBA-4DE1-AD54-97B5A7CF9E2A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -7983,7 +8023,7 @@
             <xdr:cNvPr id="8" name="CaixaDeTexto 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{46ABD740-64F5-4D1A-9170-F2C081C5D1FF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{46ABD740-64F5-4D1A-9170-F2C081C5D1FF}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -8546,7 +8586,7 @@
             <xdr:cNvPr id="9" name="CaixaDeTexto 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFA70203-3F0B-4914-9B75-03B6673FB4B6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CFA70203-3F0B-4914-9B75-03B6673FB4B6}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9061,7 +9101,7 @@
             <xdr:cNvPr id="10" name="CaixaDeTexto 9">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B1E8FE8-DDAE-4A7B-860E-55E937691175}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{1B1E8FE8-DDAE-4A7B-860E-55E937691175}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -9627,7 +9667,7 @@
         <xdr:cNvPr id="7" name="Gráfico 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F33125E0-6770-464B-AE81-F5AECA1084D6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{F33125E0-6770-464B-AE81-F5AECA1084D6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9663,7 +9703,7 @@
         <xdr:cNvPr id="11" name="Gráfico 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08229CFF-CECC-48DE-B8C8-FEE6B5EBFA07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{08229CFF-CECC-48DE-B8C8-FEE6B5EBFA07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9701,7 +9741,7 @@
         <xdr:cNvPr id="12" name="Gráfico 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF29F8FD-F73E-4C70-AC08-9EF170C82E58}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{FF29F8FD-F73E-4C70-AC08-9EF170C82E58}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -9986,11 +10026,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{873257D0-61F5-421C-B639-672E7A5240C0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L56" sqref="L56"/>
+    <sheetView tabSelected="1" topLeftCell="I4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10016,55 +10056,55 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39"/>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="45"/>
-      <c r="Q1" s="52"/>
-      <c r="R1" s="80"/>
-      <c r="S1" s="79"/>
-      <c r="T1" s="79"/>
-      <c r="U1" s="79"/>
-      <c r="V1" s="79"/>
-      <c r="W1" s="79"/>
-      <c r="X1" s="79"/>
-      <c r="Y1" s="79"/>
-      <c r="Z1" s="38"/>
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="44"/>
+      <c r="Q1" s="51"/>
+      <c r="R1" s="77"/>
+      <c r="S1" s="76"/>
+      <c r="T1" s="76"/>
+      <c r="U1" s="76"/>
+      <c r="V1" s="76"/>
+      <c r="W1" s="76"/>
+      <c r="X1" s="76"/>
+      <c r="Y1" s="76"/>
+      <c r="Z1" s="37"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="45"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="44"/>
       <c r="Q2" s="7"/>
       <c r="R2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="S2" s="87">
+      <c r="S2" s="84">
         <v>9000000</v>
       </c>
       <c r="T2" s="3"/>
@@ -10073,28 +10113,28 @@
       <c r="W2" s="3"/>
       <c r="X2" s="3"/>
       <c r="Y2" s="4"/>
-      <c r="Z2" s="38"/>
+      <c r="Z2" s="37"/>
     </row>
     <row r="3" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="45"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="38"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="38"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="38"/>
+      <c r="M3" s="38"/>
+      <c r="N3" s="38"/>
+      <c r="O3" s="38"/>
+      <c r="P3" s="44"/>
       <c r="Q3" s="7"/>
-      <c r="R3" s="42" t="s">
-        <v>25</v>
+      <c r="R3" s="41" t="s">
+        <v>24</v>
       </c>
       <c r="S3" s="5">
         <v>0.64</v>
@@ -10107,25 +10147,25 @@
       <c r="Y3" s="7"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
-      <c r="M4" s="39"/>
-      <c r="N4" s="39"/>
-      <c r="O4" s="39"/>
-      <c r="P4" s="45"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
+      <c r="K4" s="38"/>
+      <c r="L4" s="38"/>
+      <c r="M4" s="38"/>
+      <c r="N4" s="38"/>
+      <c r="O4" s="38"/>
+      <c r="P4" s="44"/>
       <c r="Q4" s="7"/>
-      <c r="R4" s="42" t="s">
-        <v>26</v>
+      <c r="R4" s="41" t="s">
+        <v>25</v>
       </c>
       <c r="S4" s="5">
         <v>0.36</v>
@@ -10136,28 +10176,28 @@
       <c r="W4" s="6"/>
       <c r="X4" s="6"/>
       <c r="Y4" s="7"/>
-      <c r="Z4" s="40"/>
+      <c r="Z4" s="39"/>
     </row>
     <row r="5" spans="1:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="39"/>
-      <c r="O5" s="39"/>
-      <c r="P5" s="45"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
+      <c r="F5" s="38"/>
+      <c r="G5" s="38"/>
+      <c r="H5" s="38"/>
+      <c r="I5" s="38"/>
+      <c r="J5" s="38"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="38"/>
+      <c r="O5" s="38"/>
+      <c r="P5" s="44"/>
       <c r="Q5" s="7"/>
-      <c r="R5" s="42" t="s">
-        <v>27</v>
+      <c r="R5" s="41" t="s">
+        <v>26</v>
       </c>
       <c r="S5" s="5">
         <v>0.23</v>
@@ -10168,28 +10208,28 @@
       <c r="W5" s="6"/>
       <c r="X5" s="6"/>
       <c r="Y5" s="7"/>
-      <c r="Z5" s="40"/>
+      <c r="Z5" s="39"/>
     </row>
     <row r="6" spans="1:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
-      <c r="M6" s="39"/>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
-      <c r="P6" s="45"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="38"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+      <c r="J6" s="38"/>
+      <c r="K6" s="38"/>
+      <c r="L6" s="38"/>
+      <c r="M6" s="38"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
+      <c r="P6" s="44"/>
       <c r="Q6" s="7"/>
-      <c r="R6" s="42" t="s">
-        <v>28</v>
+      <c r="R6" s="41" t="s">
+        <v>27</v>
       </c>
       <c r="S6" s="5">
         <v>0.31</v>
@@ -10200,30 +10240,30 @@
       <c r="W6" s="6"/>
       <c r="X6" s="6"/>
       <c r="Y6" s="7"/>
-      <c r="Z6" s="40"/>
+      <c r="Z6" s="39"/>
     </row>
     <row r="7" spans="1:26" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="39"/>
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="39"/>
-      <c r="I7" s="39"/>
-      <c r="J7" s="39"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="39"/>
-      <c r="M7" s="39"/>
-      <c r="N7" s="39"/>
-      <c r="O7" s="39"/>
-      <c r="P7" s="45"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="38"/>
+      <c r="O7" s="38"/>
+      <c r="P7" s="44"/>
       <c r="Q7" s="7"/>
-      <c r="R7" s="42" t="s">
+      <c r="R7" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="S7" s="86">
+      <c r="S7" s="83">
         <f>S2*15%</f>
         <v>1350000</v>
       </c>
@@ -10233,28 +10273,28 @@
       <c r="W7" s="6"/>
       <c r="X7" s="6"/>
       <c r="Y7" s="7"/>
-      <c r="Z7" s="40"/>
+      <c r="Z7" s="39"/>
     </row>
     <row r="8" spans="1:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="39"/>
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-      <c r="D8" s="39"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="39"/>
-      <c r="I8" s="39"/>
-      <c r="J8" s="39"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="39"/>
-      <c r="M8" s="39"/>
-      <c r="N8" s="39"/>
-      <c r="O8" s="39"/>
-      <c r="P8" s="45"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="38"/>
+      <c r="C8" s="38"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="38"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="38"/>
+      <c r="O8" s="38"/>
+      <c r="P8" s="44"/>
       <c r="Q8" s="7"/>
-      <c r="R8" s="42" t="s">
-        <v>29</v>
+      <c r="R8" s="41" t="s">
+        <v>28</v>
       </c>
       <c r="S8" s="9">
         <f>TRUNC(D22+(((G30/2)-J21)/H22)*(F22-D22),0)</f>
@@ -10264,42 +10304,42 @@
       <c r="U8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="V8" s="83">
+      <c r="V8" s="80">
         <f>L22*8/22</f>
         <v>7057521.9501465596</v>
       </c>
       <c r="W8" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="X8" s="83">
+      <c r="X8" s="80">
         <f>N22*8/22</f>
         <v>520845.11992081621</v>
       </c>
       <c r="Y8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Z8" s="40"/>
+      <c r="Z8" s="39"/>
     </row>
     <row r="9" spans="1:26" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39"/>
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="39"/>
-      <c r="J9" s="39"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="39"/>
-      <c r="M9" s="39"/>
-      <c r="N9" s="39"/>
-      <c r="O9" s="39"/>
-      <c r="P9" s="45"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="38"/>
+      <c r="K9" s="38"/>
+      <c r="L9" s="38"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="38"/>
+      <c r="O9" s="38"/>
+      <c r="P9" s="44"/>
       <c r="Q9" s="7"/>
-      <c r="R9" s="42" t="s">
-        <v>30</v>
+      <c r="R9" s="41" t="s">
+        <v>29</v>
       </c>
       <c r="S9" s="9">
         <f>TRUNC(D41+(((G48/2)-J39)/H41)*(F41-D41))</f>
@@ -10309,77 +10349,77 @@
       <c r="U9" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="V9" s="84">
+      <c r="V9" s="81">
         <f>L40*8/22</f>
         <v>3969856.0969574405</v>
       </c>
       <c r="W9" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="X9" s="84">
+      <c r="X9" s="81">
         <f>N40*8/22</f>
         <v>292975.37995545915</v>
       </c>
       <c r="Y9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Z9" s="40"/>
+      <c r="Z9" s="39"/>
     </row>
     <row r="10" spans="1:26" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="39"/>
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-      <c r="D10" s="39"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="39"/>
-      <c r="J10" s="39"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="39"/>
-      <c r="M10" s="39"/>
-      <c r="N10" s="39"/>
-      <c r="O10" s="39"/>
-      <c r="P10" s="45"/>
+      <c r="A10" s="38"/>
+      <c r="B10" s="38"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
+      <c r="F10" s="38"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="38"/>
+      <c r="I10" s="38"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="38"/>
+      <c r="L10" s="38"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="38"/>
+      <c r="O10" s="38"/>
+      <c r="P10" s="44"/>
       <c r="Q10" s="7"/>
-      <c r="R10" s="43" t="s">
-        <v>31</v>
+      <c r="R10" s="42" t="s">
+        <v>30</v>
       </c>
       <c r="S10" s="9"/>
       <c r="T10" s="6"/>
-      <c r="V10" s="81">
+      <c r="V10" s="78">
         <f xml:space="preserve"> V8/V9</f>
         <v>1.7777777777777775</v>
       </c>
-      <c r="W10" s="82"/>
-      <c r="X10" s="81">
+      <c r="W10" s="79"/>
+      <c r="X10" s="78">
         <f>X8/X9</f>
         <v>1.7777777777777777</v>
       </c>
       <c r="Y10" s="7"/>
-      <c r="Z10" s="40"/>
+      <c r="Z10" s="39"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="39"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="39"/>
-      <c r="J11" s="39"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="39"/>
-      <c r="O11" s="39"/>
-      <c r="P11" s="45"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="40"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="40"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="38"/>
+      <c r="J11" s="38"/>
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="38"/>
+      <c r="O11" s="38"/>
+      <c r="P11" s="44"/>
       <c r="Q11" s="7"/>
-      <c r="R11" s="42" t="s">
-        <v>32</v>
+      <c r="R11" s="41" t="s">
+        <v>31</v>
       </c>
       <c r="S11" s="11" t="s">
         <v>16</v>
@@ -10387,14 +10427,14 @@
       <c r="T11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="U11" s="83">
+      <c r="U11" s="80">
         <f>L24</f>
         <v>16897309.606133547</v>
       </c>
       <c r="V11" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="W11" s="83">
+      <c r="W11" s="80">
         <f>N24</f>
         <v>1013838.5763680128</v>
       </c>
@@ -10402,28 +10442,28 @@
         <v>21</v>
       </c>
       <c r="Y11" s="7"/>
-      <c r="Z11" s="40"/>
+      <c r="Z11" s="39"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="39"/>
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="39"/>
-      <c r="J12" s="39"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="39"/>
-      <c r="M12" s="39"/>
-      <c r="N12" s="39"/>
-      <c r="O12" s="39"/>
-      <c r="P12" s="45"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="38"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="40"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="40"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="38"/>
+      <c r="J12" s="38"/>
+      <c r="K12" s="38"/>
+      <c r="L12" s="38"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="38"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="44"/>
       <c r="Q12" s="7"/>
-      <c r="R12" s="42" t="s">
-        <v>33</v>
+      <c r="R12" s="41" t="s">
+        <v>32</v>
       </c>
       <c r="S12" s="11" t="s">
         <v>16</v>
@@ -10431,14 +10471,14 @@
       <c r="T12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="U12" s="83">
+      <c r="U12" s="80">
         <f>L42</f>
         <v>9504736.6534501221</v>
       </c>
       <c r="V12" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="W12" s="83">
+      <c r="W12" s="80">
         <f>N42</f>
         <v>570284.1992070073</v>
       </c>
@@ -10446,28 +10486,28 @@
         <v>21</v>
       </c>
       <c r="Y12" s="7"/>
-      <c r="Z12" s="40"/>
+      <c r="Z12" s="39"/>
     </row>
     <row r="13" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="39"/>
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="39"/>
-      <c r="J13" s="39"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="39"/>
-      <c r="M13" s="39"/>
-      <c r="N13" s="39"/>
-      <c r="O13" s="39"/>
-      <c r="P13" s="45"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="40"/>
+      <c r="E13" s="40"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="40"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="38"/>
+      <c r="O13" s="38"/>
+      <c r="P13" s="44"/>
       <c r="Q13" s="7"/>
       <c r="R13" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S13" s="13" t="s">
         <v>16</v>
@@ -10475,14 +10515,14 @@
       <c r="T13" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="U13" s="85">
+      <c r="U13" s="82">
         <f>L61</f>
         <v>17176480.893392783</v>
       </c>
       <c r="V13" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="W13" s="85">
+      <c r="W13" s="82">
         <f>N61</f>
         <v>2061177.7072071338</v>
       </c>
@@ -10490,107 +10530,107 @@
         <v>21</v>
       </c>
       <c r="Y13" s="15"/>
-      <c r="Z13" s="40"/>
+      <c r="Z13" s="39"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" s="39"/>
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="39"/>
-      <c r="J14" s="39"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="39"/>
-      <c r="M14" s="39"/>
-      <c r="N14" s="39"/>
-      <c r="O14" s="39"/>
-      <c r="P14" s="39"/>
-      <c r="Q14" s="34"/>
-      <c r="R14" s="35"/>
-      <c r="S14" s="36"/>
-      <c r="T14" s="37"/>
-      <c r="U14" s="37"/>
-      <c r="V14" s="37"/>
-      <c r="W14" s="37"/>
-      <c r="X14" s="37"/>
-      <c r="Y14" s="37"/>
-      <c r="Z14" s="37"/>
+      <c r="A14" s="38"/>
+      <c r="B14" s="38"/>
+      <c r="C14" s="38"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="38"/>
+      <c r="J14" s="38"/>
+      <c r="K14" s="38"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="38"/>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="33"/>
+      <c r="R14" s="34"/>
+      <c r="S14" s="35"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="36"/>
+      <c r="V14" s="36"/>
+      <c r="W14" s="36"/>
+      <c r="X14" s="36"/>
+      <c r="Y14" s="36"/>
+      <c r="Z14" s="36"/>
     </row>
     <row r="15" spans="1:26" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="44"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="114" t="s">
+      <c r="A15" s="43"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="118" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="115"/>
-      <c r="E15" s="115"/>
-      <c r="F15" s="115"/>
-      <c r="G15" s="115"/>
-      <c r="H15" s="115"/>
-      <c r="I15" s="115"/>
-      <c r="J15" s="115"/>
-      <c r="K15" s="115"/>
-      <c r="L15" s="115"/>
-      <c r="M15" s="115"/>
-      <c r="N15" s="115"/>
-      <c r="O15" s="115"/>
-      <c r="P15" s="116"/>
-      <c r="Q15" s="46"/>
-      <c r="R15" s="47"/>
-      <c r="S15" s="48"/>
-      <c r="T15" s="44"/>
-      <c r="U15" s="44"/>
-      <c r="V15" s="44"/>
-      <c r="W15" s="44"/>
-      <c r="X15" s="44"/>
-      <c r="Y15" s="44"/>
-      <c r="Z15" s="44"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+      <c r="F15" s="119"/>
+      <c r="G15" s="119"/>
+      <c r="H15" s="119"/>
+      <c r="I15" s="119"/>
+      <c r="J15" s="119"/>
+      <c r="K15" s="119"/>
+      <c r="L15" s="119"/>
+      <c r="M15" s="119"/>
+      <c r="N15" s="119"/>
+      <c r="O15" s="119"/>
+      <c r="P15" s="120"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="46"/>
+      <c r="S15" s="47"/>
+      <c r="T15" s="43"/>
+      <c r="U15" s="43"/>
+      <c r="V15" s="43"/>
+      <c r="W15" s="43"/>
+      <c r="X15" s="43"/>
+      <c r="Y15" s="43"/>
+      <c r="Z15" s="43"/>
     </row>
     <row r="16" spans="1:26" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="6"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="124" t="s">
+      <c r="B16" s="51"/>
+      <c r="C16" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="D16" s="122" t="s">
+      <c r="D16" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="122"/>
-      <c r="F16" s="122"/>
-      <c r="G16" s="124" t="s">
+      <c r="E16" s="112"/>
+      <c r="F16" s="112"/>
+      <c r="G16" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="H16" s="122" t="s">
+      <c r="H16" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="122" t="s">
+      <c r="I16" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="J16" s="122" t="s">
+      <c r="J16" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="K16" s="122" t="s">
+      <c r="K16" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="L16" s="122" t="s">
+      <c r="L16" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="M16" s="122" t="s">
+      <c r="M16" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="N16" s="122" t="s">
+      <c r="N16" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="O16" s="126" t="s">
+      <c r="O16" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="P16" s="126"/>
-      <c r="Q16" s="53"/>
-      <c r="R16" s="49"/>
+      <c r="P16" s="111"/>
+      <c r="Q16" s="52"/>
+      <c r="R16" s="48"/>
       <c r="S16" s="8"/>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
@@ -10602,30 +10642,30 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="128"/>
-      <c r="D17" s="56" t="s">
+      <c r="B17" s="51"/>
+      <c r="C17" s="115"/>
+      <c r="D17" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="E17" s="57"/>
-      <c r="F17" s="56" t="s">
+      <c r="E17" s="135"/>
+      <c r="F17" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="G17" s="128"/>
-      <c r="H17" s="127"/>
-      <c r="I17" s="127"/>
-      <c r="J17" s="127"/>
-      <c r="K17" s="127"/>
-      <c r="L17" s="127"/>
-      <c r="M17" s="127"/>
-      <c r="N17" s="127"/>
-      <c r="O17" s="54" t="s">
+      <c r="G17" s="115"/>
+      <c r="H17" s="113"/>
+      <c r="I17" s="113"/>
+      <c r="J17" s="113"/>
+      <c r="K17" s="113"/>
+      <c r="L17" s="113"/>
+      <c r="M17" s="113"/>
+      <c r="N17" s="113"/>
+      <c r="O17" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="P17" s="54" t="s">
+      <c r="P17" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="Q17" s="53"/>
+      <c r="Q17" s="52"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
       <c r="T17" s="6"/>
@@ -10636,67 +10676,67 @@
       <c r="Y17" s="6"/>
       <c r="Z17" s="6"/>
     </row>
-    <row r="18" spans="1:26" s="108" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="96"/>
-      <c r="B18" s="97"/>
-      <c r="C18" s="98">
+    <row r="18" spans="1:26" s="105" customFormat="1" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="93"/>
+      <c r="B18" s="94"/>
+      <c r="C18" s="95">
         <v>1</v>
       </c>
-      <c r="D18" s="99">
+      <c r="D18" s="126">
         <v>1</v>
       </c>
-      <c r="E18" s="99" t="s">
+      <c r="E18" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="99">
+      <c r="F18" s="127">
         <v>31</v>
       </c>
-      <c r="G18" s="100">
+      <c r="G18" s="97">
         <f>(F18-D18)/2</f>
         <v>15</v>
       </c>
-      <c r="H18" s="100">
+      <c r="H18" s="97">
         <v>22</v>
       </c>
-      <c r="I18" s="101">
+      <c r="I18" s="98">
         <f t="shared" ref="I18:I29" si="0">H18/$H$30</f>
         <v>8.6274509803921567E-2</v>
       </c>
-      <c r="J18" s="100">
+      <c r="J18" s="97">
         <v>22</v>
       </c>
-      <c r="K18" s="102">
+      <c r="K18" s="99">
         <f>I18</f>
         <v>8.6274509803921567E-2</v>
       </c>
-      <c r="L18" s="103">
+      <c r="L18" s="100">
         <f>S2*S3* 4.38</f>
         <v>25228800</v>
       </c>
-      <c r="M18" s="102">
+      <c r="M18" s="99">
         <v>0.06</v>
       </c>
-      <c r="N18" s="104">
+      <c r="N18" s="101">
         <f>L18*M18</f>
         <v>1513728</v>
       </c>
-      <c r="O18" s="105"/>
-      <c r="P18" s="106"/>
-      <c r="Q18" s="96"/>
-      <c r="R18" s="96"/>
-      <c r="S18" s="96"/>
-      <c r="T18" s="96"/>
-      <c r="U18" s="96"/>
-      <c r="V18" s="96"/>
-      <c r="W18" s="96"/>
-      <c r="X18" s="107"/>
-      <c r="Y18" s="96"/>
-      <c r="Z18" s="96"/>
+      <c r="O18" s="102"/>
+      <c r="P18" s="103"/>
+      <c r="Q18" s="93"/>
+      <c r="R18" s="93"/>
+      <c r="S18" s="93"/>
+      <c r="T18" s="93"/>
+      <c r="U18" s="93"/>
+      <c r="V18" s="93"/>
+      <c r="W18" s="93"/>
+      <c r="X18" s="104"/>
+      <c r="Y18" s="93"/>
+      <c r="Z18" s="93"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="59">
+      <c r="B19" s="51"/>
+      <c r="C19" s="56">
         <v>2</v>
       </c>
       <c r="D19" s="19">
@@ -10727,20 +10767,20 @@
         <f>I19+K18</f>
         <v>0.16470588235294117</v>
       </c>
-      <c r="L19" s="83">
+      <c r="L19" s="80">
         <f>L18-N18</f>
         <v>23715072</v>
       </c>
       <c r="M19" s="24">
         <v>0.06</v>
       </c>
-      <c r="N19" s="88">
+      <c r="N19" s="85">
         <f>L19*M19</f>
         <v>1422904.3199999998</v>
       </c>
-      <c r="O19" s="76"/>
+      <c r="O19" s="73"/>
       <c r="P19" s="27"/>
-      <c r="Q19" s="50"/>
+      <c r="Q19" s="49"/>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
@@ -10753,8 +10793,8 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="6"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="59">
+      <c r="B20" s="51"/>
+      <c r="C20" s="56">
         <v>3</v>
       </c>
       <c r="D20" s="19">
@@ -10785,26 +10825,26 @@
         <f t="shared" ref="K20:K29" si="3">I20+K19</f>
         <v>0.24313725490196078</v>
       </c>
-      <c r="L20" s="83">
+      <c r="L20" s="80">
         <f t="shared" ref="L20:L29" si="4">L19-N19</f>
         <v>22292167.68</v>
       </c>
       <c r="M20" s="24">
         <v>0.06</v>
       </c>
-      <c r="N20" s="89">
+      <c r="N20" s="86">
         <f t="shared" ref="N20:N29" si="5">L20*M20</f>
         <v>1337530.0607999999</v>
       </c>
-      <c r="O20" s="93">
+      <c r="O20" s="90">
         <f>AVERAGE(L18:L20)</f>
         <v>23745346.560000002</v>
       </c>
-      <c r="P20" s="93">
+      <c r="P20" s="90">
         <f>AVERAGE(N18:N20)</f>
         <v>1424720.7935999997</v>
       </c>
-      <c r="Q20" s="53"/>
+      <c r="Q20" s="52"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
       <c r="T20" s="6"/>
@@ -10817,8 +10857,8 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="6"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="59">
+      <c r="B21" s="51"/>
+      <c r="C21" s="56">
         <v>4</v>
       </c>
       <c r="D21" s="19">
@@ -10849,18 +10889,18 @@
         <f t="shared" si="3"/>
         <v>0.32549019607843138</v>
       </c>
-      <c r="L21" s="83">
+      <c r="L21" s="80">
         <f t="shared" si="4"/>
         <v>20954637.619199999</v>
       </c>
       <c r="M21" s="24">
         <v>7.3800000000000004E-2</v>
       </c>
-      <c r="N21" s="88">
+      <c r="N21" s="85">
         <f t="shared" si="5"/>
         <v>1546452.2562969599</v>
       </c>
-      <c r="O21" s="55"/>
+      <c r="O21" s="54"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
@@ -10875,8 +10915,8 @@
     </row>
     <row r="22" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="59">
+      <c r="B22" s="51"/>
+      <c r="C22" s="56">
         <v>5</v>
       </c>
       <c r="D22" s="19">
@@ -10907,18 +10947,18 @@
         <f t="shared" si="3"/>
         <v>0.41176470588235292</v>
       </c>
-      <c r="L22" s="83">
+      <c r="L22" s="80">
         <f t="shared" si="4"/>
         <v>19408185.36290304</v>
       </c>
       <c r="M22" s="24">
         <v>7.3800000000000004E-2</v>
       </c>
-      <c r="N22" s="88">
+      <c r="N22" s="85">
         <f t="shared" si="5"/>
         <v>1432324.0797822445</v>
       </c>
-      <c r="O22" s="76"/>
+      <c r="O22" s="73"/>
       <c r="P22" s="27"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
@@ -10933,8 +10973,8 @@
     </row>
     <row r="23" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="6"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="59">
+      <c r="B23" s="51"/>
+      <c r="C23" s="56">
         <v>6</v>
       </c>
       <c r="D23" s="19">
@@ -10965,26 +11005,26 @@
         <f t="shared" si="3"/>
         <v>0.49019607843137253</v>
       </c>
-      <c r="L23" s="83">
+      <c r="L23" s="80">
         <f t="shared" si="4"/>
         <v>17975861.283120796</v>
       </c>
       <c r="M23" s="24">
         <v>0.06</v>
       </c>
-      <c r="N23" s="89">
+      <c r="N23" s="86">
         <f t="shared" si="5"/>
         <v>1078551.6769872478</v>
       </c>
-      <c r="O23" s="93">
+      <c r="O23" s="90">
         <f>AVERAGE(L21:L23)</f>
         <v>19446228.088407945</v>
       </c>
-      <c r="P23" s="93">
+      <c r="P23" s="90">
         <f>AVERAGE(N21:N23)</f>
         <v>1352442.6710221507</v>
       </c>
-      <c r="Q23" s="53"/>
+      <c r="Q23" s="52"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
@@ -10997,8 +11037,8 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="6"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="59">
+      <c r="B24" s="51"/>
+      <c r="C24" s="56">
         <v>7</v>
       </c>
       <c r="D24" s="19">
@@ -11029,18 +11069,18 @@
         <f t="shared" si="3"/>
         <v>0.58039215686274503</v>
       </c>
-      <c r="L24" s="83">
+      <c r="L24" s="80">
         <f t="shared" si="4"/>
         <v>16897309.606133547</v>
       </c>
       <c r="M24" s="24">
         <v>0.06</v>
       </c>
-      <c r="N24" s="88">
+      <c r="N24" s="85">
         <f t="shared" si="5"/>
         <v>1013838.5763680128</v>
       </c>
-      <c r="O24" s="55"/>
+      <c r="O24" s="54"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
@@ -11055,8 +11095,8 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="59">
+      <c r="B25" s="51"/>
+      <c r="C25" s="56">
         <v>8</v>
       </c>
       <c r="D25" s="19">
@@ -11087,18 +11127,18 @@
         <f t="shared" si="3"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="L25" s="83">
+      <c r="L25" s="80">
         <f t="shared" si="4"/>
         <v>15883471.029765533</v>
       </c>
       <c r="M25" s="24">
         <v>0.06</v>
       </c>
-      <c r="N25" s="88">
+      <c r="N25" s="85">
         <f t="shared" si="5"/>
         <v>953008.261785932</v>
       </c>
-      <c r="O25" s="76"/>
+      <c r="O25" s="73"/>
       <c r="P25" s="27"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
@@ -11113,8 +11153,8 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="59">
+      <c r="B26" s="51"/>
+      <c r="C26" s="56">
         <v>9</v>
       </c>
       <c r="D26" s="19">
@@ -11145,26 +11185,26 @@
         <f t="shared" si="3"/>
         <v>0.74901960784313726</v>
       </c>
-      <c r="L26" s="83">
+      <c r="L26" s="80">
         <f t="shared" si="4"/>
         <v>14930462.767979601</v>
       </c>
       <c r="M26" s="24">
         <v>0.06</v>
       </c>
-      <c r="N26" s="89">
+      <c r="N26" s="86">
         <f t="shared" si="5"/>
         <v>895827.7660787761</v>
       </c>
-      <c r="O26" s="93">
+      <c r="O26" s="90">
         <f t="shared" ref="O26" si="6">AVERAGE(L24:L26)</f>
         <v>15903747.801292894</v>
       </c>
-      <c r="P26" s="93">
+      <c r="P26" s="90">
         <f>AVERAGE(N24:N26)</f>
         <v>954224.86807757372</v>
       </c>
-      <c r="Q26" s="53"/>
+      <c r="Q26" s="52"/>
       <c r="R26" s="6"/>
       <c r="S26" s="6"/>
       <c r="T26" s="6"/>
@@ -11177,8 +11217,8 @@
     </row>
     <row r="27" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="6"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="59">
+      <c r="B27" s="51"/>
+      <c r="C27" s="56">
         <v>10</v>
       </c>
       <c r="D27" s="19">
@@ -11209,18 +11249,18 @@
         <f t="shared" si="3"/>
         <v>0.83921568627450982</v>
       </c>
-      <c r="L27" s="83">
+      <c r="L27" s="80">
         <f t="shared" si="4"/>
         <v>14034635.001900826</v>
       </c>
       <c r="M27" s="24">
         <v>0.06</v>
       </c>
-      <c r="N27" s="88">
+      <c r="N27" s="85">
         <f t="shared" si="5"/>
         <v>842078.10011404951</v>
       </c>
-      <c r="O27" s="55"/>
+      <c r="O27" s="54"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
@@ -11235,8 +11275,8 @@
     </row>
     <row r="28" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="59">
+      <c r="B28" s="51"/>
+      <c r="C28" s="56">
         <v>11</v>
       </c>
       <c r="D28" s="19">
@@ -11267,18 +11307,18 @@
         <f t="shared" si="3"/>
         <v>0.91764705882352948</v>
       </c>
-      <c r="L28" s="83">
+      <c r="L28" s="80">
         <f t="shared" si="4"/>
         <v>13192556.901786776</v>
       </c>
       <c r="M28" s="24">
         <v>0.06</v>
       </c>
-      <c r="N28" s="88">
+      <c r="N28" s="85">
         <f t="shared" si="5"/>
         <v>791553.41410720651</v>
       </c>
-      <c r="O28" s="76"/>
+      <c r="O28" s="73"/>
       <c r="P28" s="27"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
@@ -11293,17 +11333,17 @@
     </row>
     <row r="29" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="6"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="71">
+      <c r="B29" s="51"/>
+      <c r="C29" s="68">
         <v>12</v>
       </c>
-      <c r="D29" s="29">
+      <c r="D29" s="28">
         <v>1</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E29" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F29" s="31">
+      <c r="F29" s="30">
         <v>31</v>
       </c>
       <c r="G29" s="16">
@@ -11317,34 +11357,34 @@
         <f t="shared" si="0"/>
         <v>8.2352941176470587E-2</v>
       </c>
-      <c r="J29" s="32">
+      <c r="J29" s="31">
         <f t="shared" si="2"/>
         <v>255</v>
       </c>
-      <c r="K29" s="33">
+      <c r="K29" s="32">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="L29" s="84">
+      <c r="L29" s="81">
         <f t="shared" si="4"/>
         <v>12401003.487679569</v>
       </c>
-      <c r="M29" s="33">
+      <c r="M29" s="32">
         <v>7.3800000000000004E-2</v>
       </c>
-      <c r="N29" s="90">
+      <c r="N29" s="87">
         <f t="shared" si="5"/>
         <v>915194.05739075225</v>
       </c>
-      <c r="O29" s="93">
+      <c r="O29" s="90">
         <f t="shared" ref="O29" si="7">AVERAGE(L27:L29)</f>
         <v>13209398.463789059</v>
       </c>
-      <c r="P29" s="93">
+      <c r="P29" s="90">
         <f>AVERAGE(N27:N29)</f>
         <v>849608.52387066942</v>
       </c>
-      <c r="Q29" s="53"/>
+      <c r="Q29" s="52"/>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
@@ -11357,37 +11397,37 @@
     </row>
     <row r="30" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="6"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="72" t="s">
+      <c r="B30" s="51"/>
+      <c r="C30" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="D30" s="69"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="68"/>
-      <c r="G30" s="73">
+      <c r="D30" s="66"/>
+      <c r="E30" s="55"/>
+      <c r="F30" s="65"/>
+      <c r="G30" s="70">
         <f>SUBTOTAL(9,G18:G29)</f>
         <v>176.5</v>
       </c>
-      <c r="H30" s="74">
+      <c r="H30" s="71">
         <f>SUBTOTAL(9,H18:H29)</f>
         <v>255</v>
       </c>
-      <c r="I30" s="75">
+      <c r="I30" s="72">
         <f>SUBTOTAL(9,I18:I29)</f>
         <v>1</v>
       </c>
-      <c r="J30" s="69"/>
-      <c r="K30" s="68"/>
-      <c r="L30" s="91">
+      <c r="J30" s="66"/>
+      <c r="K30" s="65"/>
+      <c r="L30" s="88">
         <f>SUBTOTAL(9,L18:L29)</f>
         <v>216914162.74046969</v>
       </c>
-      <c r="M30" s="70"/>
-      <c r="N30" s="91">
+      <c r="M30" s="67"/>
+      <c r="N30" s="88">
         <f>SUBTOTAL(9,N18:N29)</f>
         <v>13742990.569711182</v>
       </c>
-      <c r="O30" s="55"/>
+      <c r="O30" s="54"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
@@ -11403,18 +11443,18 @@
     <row r="31" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6"/>
       <c r="B31" s="6"/>
-      <c r="C31" s="58"/>
+      <c r="C31" s="55"/>
       <c r="D31" s="6"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
       <c r="J31" s="6"/>
       <c r="K31" s="6"/>
-      <c r="L31" s="58"/>
+      <c r="L31" s="55"/>
       <c r="M31" s="6"/>
-      <c r="N31" s="58"/>
+      <c r="N31" s="55"/>
       <c r="O31" s="6"/>
       <c r="P31" s="6"/>
       <c r="Q31" s="6"/>
@@ -11441,11 +11481,8 @@
       <c r="J32" s="6"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
-      <c r="M32" s="51"/>
-      <c r="N32" s="6">
-        <f>LARGE(N18:N29,1)</f>
-        <v>1546452.2562969599</v>
-      </c>
+      <c r="M32" s="50"/>
+      <c r="N32" s="6"/>
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
@@ -11462,22 +11499,22 @@
     <row r="33" spans="1:26" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="6"/>
       <c r="B33" s="6"/>
-      <c r="C33" s="117" t="s">
+      <c r="C33" s="121" t="s">
         <v>23</v>
       </c>
-      <c r="D33" s="118"/>
-      <c r="E33" s="118"/>
-      <c r="F33" s="118"/>
-      <c r="G33" s="118"/>
-      <c r="H33" s="118"/>
-      <c r="I33" s="118"/>
-      <c r="J33" s="118"/>
-      <c r="K33" s="118"/>
-      <c r="L33" s="118"/>
-      <c r="M33" s="118"/>
-      <c r="N33" s="118"/>
-      <c r="O33" s="118"/>
-      <c r="P33" s="119"/>
+      <c r="D33" s="122"/>
+      <c r="E33" s="122"/>
+      <c r="F33" s="122"/>
+      <c r="G33" s="122"/>
+      <c r="H33" s="122"/>
+      <c r="I33" s="122"/>
+      <c r="J33" s="122"/>
+      <c r="K33" s="122"/>
+      <c r="L33" s="122"/>
+      <c r="M33" s="122"/>
+      <c r="N33" s="122"/>
+      <c r="O33" s="122"/>
+      <c r="P33" s="123"/>
       <c r="Q33" s="6"/>
       <c r="R33" s="6"/>
       <c r="S33" s="6"/>
@@ -11491,44 +11528,44 @@
     </row>
     <row r="34" spans="1:26" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="6"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="124" t="s">
+      <c r="B34" s="51"/>
+      <c r="C34" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="D34" s="122" t="s">
+      <c r="D34" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="122"/>
-      <c r="F34" s="122"/>
-      <c r="G34" s="124" t="s">
+      <c r="E34" s="112"/>
+      <c r="F34" s="112"/>
+      <c r="G34" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="122" t="s">
+      <c r="H34" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="I34" s="122" t="s">
+      <c r="I34" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="J34" s="122" t="s">
+      <c r="J34" s="112" t="s">
+        <v>34</v>
+      </c>
+      <c r="K34" s="112" t="s">
         <v>35</v>
       </c>
-      <c r="K34" s="122" t="s">
-        <v>36</v>
-      </c>
-      <c r="L34" s="122" t="s">
+      <c r="L34" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="M34" s="122" t="s">
+      <c r="M34" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="N34" s="122" t="s">
+      <c r="N34" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="O34" s="126" t="s">
+      <c r="O34" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="P34" s="126"/>
-      <c r="Q34" s="53"/>
+      <c r="P34" s="111"/>
+      <c r="Q34" s="52"/>
       <c r="R34" s="6"/>
       <c r="S34" s="6"/>
       <c r="T34" s="6"/>
@@ -11541,30 +11578,30 @@
     </row>
     <row r="35" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="6"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="125"/>
-      <c r="D35" s="54" t="s">
+      <c r="B35" s="51"/>
+      <c r="C35" s="116"/>
+      <c r="D35" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="E35" s="28"/>
-      <c r="F35" s="61" t="s">
+      <c r="E35" s="135"/>
+      <c r="F35" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="G35" s="125"/>
-      <c r="H35" s="123"/>
-      <c r="I35" s="123"/>
-      <c r="J35" s="123"/>
-      <c r="K35" s="123"/>
-      <c r="L35" s="123"/>
-      <c r="M35" s="123"/>
-      <c r="N35" s="123"/>
-      <c r="O35" s="61" t="s">
+      <c r="G35" s="116"/>
+      <c r="H35" s="117"/>
+      <c r="I35" s="117"/>
+      <c r="J35" s="117"/>
+      <c r="K35" s="117"/>
+      <c r="L35" s="117"/>
+      <c r="M35" s="117"/>
+      <c r="N35" s="117"/>
+      <c r="O35" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="P35" s="54" t="s">
+      <c r="P35" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="Q35" s="53"/>
+      <c r="Q35" s="52"/>
       <c r="R35" s="6"/>
       <c r="S35" s="6"/>
       <c r="T35" s="6"/>
@@ -11577,50 +11614,50 @@
     </row>
     <row r="36" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="63">
+      <c r="B36" s="51"/>
+      <c r="C36" s="60">
         <v>1</v>
       </c>
-      <c r="D36" s="64">
+      <c r="D36" s="128">
         <v>1</v>
       </c>
-      <c r="E36" s="64" t="s">
+      <c r="E36" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="F36" s="64">
+      <c r="F36" s="131">
         <v>31</v>
       </c>
-      <c r="G36" s="64">
+      <c r="G36" s="61">
         <f>(F36-D36)/2</f>
         <v>15</v>
       </c>
-      <c r="H36" s="64">
+      <c r="H36" s="61">
         <v>22</v>
       </c>
-      <c r="I36" s="65">
+      <c r="I36" s="62">
         <f t="shared" ref="I36:I47" si="8">H36/$H$30</f>
         <v>8.6274509803921567E-2</v>
       </c>
-      <c r="J36" s="64">
+      <c r="J36" s="61">
         <v>22</v>
       </c>
-      <c r="K36" s="66">
+      <c r="K36" s="63">
         <f>I36</f>
         <v>8.6274509803921567E-2</v>
       </c>
-      <c r="L36" s="92">
+      <c r="L36" s="89">
         <f>S2*S4* 4.38</f>
         <v>14191200</v>
       </c>
-      <c r="M36" s="109">
+      <c r="M36" s="106">
         <v>0.06</v>
       </c>
-      <c r="N36" s="94">
+      <c r="N36" s="91">
         <f>L36*M36</f>
         <v>851472</v>
       </c>
-      <c r="O36" s="62"/>
-      <c r="P36" s="60"/>
+      <c r="O36" s="59"/>
+      <c r="P36" s="57"/>
       <c r="Q36" s="6"/>
       <c r="R36" s="6"/>
       <c r="S36" s="6"/>
@@ -11634,17 +11671,17 @@
     </row>
     <row r="37" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="6"/>
-      <c r="B37" s="52"/>
+      <c r="B37" s="51"/>
       <c r="C37" s="18">
         <v>2</v>
       </c>
-      <c r="D37" s="22">
+      <c r="D37" s="129">
         <v>1</v>
       </c>
       <c r="E37" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F37" s="22">
+      <c r="F37" s="132">
         <v>28</v>
       </c>
       <c r="G37" s="22">
@@ -11666,19 +11703,19 @@
         <f>I37+K36</f>
         <v>0.16470588235294117</v>
       </c>
-      <c r="L37" s="83">
+      <c r="L37" s="80">
         <f>L36-N36</f>
         <v>13339728</v>
       </c>
-      <c r="M37" s="110">
+      <c r="M37" s="107">
         <v>0.06</v>
       </c>
-      <c r="N37" s="95">
+      <c r="N37" s="92">
         <f t="shared" ref="N37:N47" si="11">L37*M37</f>
         <v>800383.67999999993</v>
       </c>
-      <c r="O37" s="77"/>
-      <c r="P37" s="78"/>
+      <c r="O37" s="74"/>
+      <c r="P37" s="75"/>
       <c r="Q37" s="6"/>
       <c r="R37" s="6"/>
       <c r="S37" s="6"/>
@@ -11692,17 +11729,17 @@
     </row>
     <row r="38" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="6"/>
-      <c r="B38" s="52"/>
+      <c r="B38" s="51"/>
       <c r="C38" s="18">
         <v>3</v>
       </c>
-      <c r="D38" s="22">
+      <c r="D38" s="129">
         <v>1</v>
       </c>
       <c r="E38" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="22">
+      <c r="F38" s="132">
         <v>31</v>
       </c>
       <c r="G38" s="22">
@@ -11724,26 +11761,26 @@
         <f t="shared" ref="K38:K47" si="12">I38+K37</f>
         <v>0.24313725490196078</v>
       </c>
-      <c r="L38" s="83">
+      <c r="L38" s="80">
         <f t="shared" ref="L38:L47" si="13">L37-N37</f>
         <v>12539344.32</v>
       </c>
-      <c r="M38" s="110">
+      <c r="M38" s="107">
         <v>0.06</v>
       </c>
-      <c r="N38" s="89">
+      <c r="N38" s="86">
         <f t="shared" si="11"/>
         <v>752360.65919999999</v>
       </c>
-      <c r="O38" s="93">
+      <c r="O38" s="90">
         <f>AVERAGE(L36:L38)</f>
         <v>13356757.439999999</v>
       </c>
-      <c r="P38" s="93">
+      <c r="P38" s="90">
         <f>AVERAGE(N36:N38)</f>
         <v>801405.4463999999</v>
       </c>
-      <c r="Q38" s="53"/>
+      <c r="Q38" s="52"/>
       <c r="R38" s="6"/>
       <c r="S38" s="6"/>
       <c r="T38" s="6"/>
@@ -11756,17 +11793,17 @@
     </row>
     <row r="39" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="6"/>
-      <c r="B39" s="52"/>
+      <c r="B39" s="51"/>
       <c r="C39" s="18">
         <v>4</v>
       </c>
-      <c r="D39" s="22">
+      <c r="D39" s="129">
         <v>1</v>
       </c>
       <c r="E39" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F39" s="22">
+      <c r="F39" s="132">
         <v>30</v>
       </c>
       <c r="G39" s="22">
@@ -11788,19 +11825,19 @@
         <f t="shared" si="12"/>
         <v>0.32549019607843138</v>
       </c>
-      <c r="L39" s="83">
+      <c r="L39" s="80">
         <f t="shared" si="13"/>
         <v>11786983.660800001</v>
       </c>
-      <c r="M39" s="110">
+      <c r="M39" s="107">
         <v>7.3800000000000004E-2</v>
       </c>
-      <c r="N39" s="95">
+      <c r="N39" s="92">
         <f t="shared" si="11"/>
         <v>869879.39416704013</v>
       </c>
-      <c r="O39" s="62"/>
-      <c r="P39" s="60"/>
+      <c r="O39" s="59"/>
+      <c r="P39" s="57"/>
       <c r="Q39" s="6"/>
       <c r="R39" s="6"/>
       <c r="S39" s="6"/>
@@ -11814,17 +11851,17 @@
     </row>
     <row r="40" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="6"/>
-      <c r="B40" s="52"/>
+      <c r="B40" s="51"/>
       <c r="C40" s="18">
         <v>5</v>
       </c>
-      <c r="D40" s="22">
+      <c r="D40" s="129">
         <v>1</v>
       </c>
       <c r="E40" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F40" s="22">
+      <c r="F40" s="132">
         <v>31</v>
       </c>
       <c r="G40" s="22">
@@ -11846,19 +11883,19 @@
         <f t="shared" si="12"/>
         <v>0.41176470588235292</v>
       </c>
-      <c r="L40" s="83">
+      <c r="L40" s="80">
         <f t="shared" si="13"/>
         <v>10917104.266632961</v>
       </c>
-      <c r="M40" s="110">
+      <c r="M40" s="107">
         <v>7.3800000000000004E-2</v>
       </c>
-      <c r="N40" s="95">
+      <c r="N40" s="92">
         <f t="shared" si="11"/>
         <v>805682.29487751261</v>
       </c>
-      <c r="O40" s="77"/>
-      <c r="P40" s="78"/>
+      <c r="O40" s="74"/>
+      <c r="P40" s="75"/>
       <c r="Q40" s="6"/>
       <c r="R40" s="6"/>
       <c r="S40" s="6"/>
@@ -11872,17 +11909,17 @@
     </row>
     <row r="41" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="6"/>
-      <c r="B41" s="52"/>
+      <c r="B41" s="51"/>
       <c r="C41" s="18">
         <v>6</v>
       </c>
-      <c r="D41" s="22">
+      <c r="D41" s="129">
         <v>1</v>
       </c>
       <c r="E41" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F41" s="22">
+      <c r="F41" s="132">
         <v>30</v>
       </c>
       <c r="G41" s="22">
@@ -11904,26 +11941,26 @@
         <f t="shared" si="12"/>
         <v>0.49019607843137253</v>
       </c>
-      <c r="L41" s="83">
+      <c r="L41" s="80">
         <f t="shared" si="13"/>
         <v>10111421.971755449</v>
       </c>
-      <c r="M41" s="110">
+      <c r="M41" s="107">
         <v>0.06</v>
       </c>
-      <c r="N41" s="89">
+      <c r="N41" s="86">
         <f t="shared" si="11"/>
         <v>606685.31830532686</v>
       </c>
-      <c r="O41" s="93">
+      <c r="O41" s="90">
         <f t="shared" ref="O41" si="14">AVERAGE(L39:L41)</f>
         <v>10938503.29972947</v>
       </c>
-      <c r="P41" s="93">
+      <c r="P41" s="90">
         <f>AVERAGE(N39:N41)</f>
         <v>760749.00244995987</v>
       </c>
-      <c r="Q41" s="53"/>
+      <c r="Q41" s="52"/>
       <c r="R41" s="6"/>
       <c r="S41" s="6"/>
       <c r="T41" s="6"/>
@@ -11936,17 +11973,17 @@
     </row>
     <row r="42" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="6"/>
-      <c r="B42" s="52"/>
+      <c r="B42" s="51"/>
       <c r="C42" s="18">
         <v>7</v>
       </c>
-      <c r="D42" s="22">
+      <c r="D42" s="129">
         <v>1</v>
       </c>
       <c r="E42" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F42" s="22">
+      <c r="F42" s="132">
         <v>31</v>
       </c>
       <c r="G42" s="22">
@@ -11968,18 +12005,18 @@
         <f t="shared" si="12"/>
         <v>0.58039215686274503</v>
       </c>
-      <c r="L42" s="83">
+      <c r="L42" s="80">
         <f t="shared" si="13"/>
         <v>9504736.6534501221</v>
       </c>
-      <c r="M42" s="110">
+      <c r="M42" s="107">
         <v>0.06</v>
       </c>
-      <c r="N42" s="95">
+      <c r="N42" s="92">
         <f t="shared" si="11"/>
         <v>570284.1992070073</v>
       </c>
-      <c r="O42" s="55"/>
+      <c r="O42" s="54"/>
       <c r="P42" s="17"/>
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
@@ -11994,17 +12031,17 @@
     </row>
     <row r="43" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="6"/>
-      <c r="B43" s="52"/>
+      <c r="B43" s="51"/>
       <c r="C43" s="18">
         <v>8</v>
       </c>
-      <c r="D43" s="22">
+      <c r="D43" s="129">
         <v>1</v>
       </c>
       <c r="E43" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F43" s="22">
+      <c r="F43" s="132">
         <v>31</v>
       </c>
       <c r="G43" s="22">
@@ -12026,18 +12063,18 @@
         <f t="shared" si="12"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="L43" s="83">
+      <c r="L43" s="80">
         <f t="shared" si="13"/>
         <v>8934452.4542431142</v>
       </c>
-      <c r="M43" s="110">
+      <c r="M43" s="107">
         <v>0.06</v>
       </c>
-      <c r="N43" s="95">
+      <c r="N43" s="92">
         <f t="shared" si="11"/>
         <v>536067.1472545868</v>
       </c>
-      <c r="O43" s="76"/>
+      <c r="O43" s="73"/>
       <c r="P43" s="27"/>
       <c r="Q43" s="6"/>
       <c r="R43" s="6"/>
@@ -12052,17 +12089,17 @@
     </row>
     <row r="44" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="6"/>
-      <c r="B44" s="52"/>
+      <c r="B44" s="51"/>
       <c r="C44" s="18">
         <v>9</v>
       </c>
-      <c r="D44" s="22">
+      <c r="D44" s="129">
         <v>1</v>
       </c>
       <c r="E44" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F44" s="22">
+      <c r="F44" s="132">
         <v>30</v>
       </c>
       <c r="G44" s="22">
@@ -12084,26 +12121,26 @@
         <f t="shared" si="12"/>
         <v>0.74901960784313726</v>
       </c>
-      <c r="L44" s="83">
+      <c r="L44" s="80">
         <f t="shared" si="13"/>
         <v>8398385.306988528</v>
       </c>
-      <c r="M44" s="110">
+      <c r="M44" s="107">
         <v>0.06</v>
       </c>
-      <c r="N44" s="89">
+      <c r="N44" s="86">
         <f t="shared" si="11"/>
         <v>503903.11841931165</v>
       </c>
-      <c r="O44" s="93">
+      <c r="O44" s="90">
         <f t="shared" ref="O44" si="15">AVERAGE(L42:L44)</f>
         <v>8945858.1382272542</v>
       </c>
-      <c r="P44" s="93">
+      <c r="P44" s="90">
         <f>AVERAGE(N42:N44)</f>
         <v>536751.48829363531</v>
       </c>
-      <c r="Q44" s="53"/>
+      <c r="Q44" s="52"/>
       <c r="R44" s="6"/>
       <c r="S44" s="6"/>
       <c r="T44" s="6"/>
@@ -12116,17 +12153,17 @@
     </row>
     <row r="45" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="6"/>
-      <c r="B45" s="52"/>
+      <c r="B45" s="51"/>
       <c r="C45" s="18">
         <v>10</v>
       </c>
-      <c r="D45" s="22">
+      <c r="D45" s="129">
         <v>1</v>
       </c>
       <c r="E45" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F45" s="22">
+      <c r="F45" s="132">
         <v>31</v>
       </c>
       <c r="G45" s="22">
@@ -12148,18 +12185,18 @@
         <f t="shared" si="12"/>
         <v>0.83921568627450982</v>
       </c>
-      <c r="L45" s="83">
+      <c r="L45" s="80">
         <f t="shared" si="13"/>
         <v>7894482.1885692161</v>
       </c>
-      <c r="M45" s="110">
+      <c r="M45" s="107">
         <v>0.06</v>
       </c>
-      <c r="N45" s="95">
+      <c r="N45" s="92">
         <f t="shared" si="11"/>
         <v>473668.93131415296</v>
       </c>
-      <c r="O45" s="55"/>
+      <c r="O45" s="54"/>
       <c r="P45" s="17"/>
       <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
@@ -12174,17 +12211,17 @@
     </row>
     <row r="46" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="6"/>
-      <c r="B46" s="52"/>
+      <c r="B46" s="51"/>
       <c r="C46" s="18">
         <v>11</v>
       </c>
-      <c r="D46" s="22">
+      <c r="D46" s="129">
         <v>1</v>
       </c>
       <c r="E46" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F46" s="22">
+      <c r="F46" s="132">
         <v>30</v>
       </c>
       <c r="G46" s="22">
@@ -12206,18 +12243,18 @@
         <f t="shared" si="12"/>
         <v>0.91764705882352948</v>
       </c>
-      <c r="L46" s="83">
+      <c r="L46" s="80">
         <f t="shared" si="13"/>
         <v>7420813.2572550634</v>
       </c>
-      <c r="M46" s="110">
+      <c r="M46" s="107">
         <v>0.06</v>
       </c>
-      <c r="N46" s="95">
+      <c r="N46" s="92">
         <f t="shared" si="11"/>
         <v>445248.79543530376</v>
       </c>
-      <c r="O46" s="76"/>
+      <c r="O46" s="73"/>
       <c r="P46" s="27"/>
       <c r="Q46" s="6"/>
       <c r="R46" s="6"/>
@@ -12232,17 +12269,17 @@
     </row>
     <row r="47" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="6"/>
-      <c r="B47" s="52"/>
+      <c r="B47" s="51"/>
       <c r="C47" s="25">
         <v>12</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="130">
         <v>1</v>
       </c>
       <c r="E47" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F47" s="1">
+      <c r="F47" s="133">
         <v>31</v>
       </c>
       <c r="G47" s="16">
@@ -12260,30 +12297,30 @@
         <f t="shared" si="10"/>
         <v>255</v>
       </c>
-      <c r="K47" s="67">
+      <c r="K47" s="64">
         <f t="shared" si="12"/>
         <v>1</v>
       </c>
-      <c r="L47" s="84">
+      <c r="L47" s="81">
         <f t="shared" si="13"/>
         <v>6975564.4618197596</v>
       </c>
-      <c r="M47" s="67">
+      <c r="M47" s="64">
         <v>7.3800000000000004E-2</v>
       </c>
-      <c r="N47" s="90">
+      <c r="N47" s="87">
         <f t="shared" si="11"/>
         <v>514796.65728229831</v>
       </c>
-      <c r="O47" s="93">
+      <c r="O47" s="90">
         <f t="shared" ref="O47" si="16">AVERAGE(L45:L47)</f>
         <v>7430286.6358813467</v>
       </c>
-      <c r="P47" s="93">
+      <c r="P47" s="90">
         <f>AVERAGE(N45:N47)</f>
         <v>477904.79467725166</v>
       </c>
-      <c r="Q47" s="53"/>
+      <c r="Q47" s="52"/>
       <c r="R47" s="6"/>
       <c r="S47" s="6"/>
       <c r="T47" s="6"/>
@@ -12296,38 +12333,38 @@
     </row>
     <row r="48" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="6"/>
-      <c r="B48" s="52"/>
-      <c r="C48" s="72" t="s">
+      <c r="B48" s="51"/>
+      <c r="C48" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="D48" s="69"/>
-      <c r="E48" s="58"/>
-      <c r="F48" s="68"/>
-      <c r="G48" s="73">
+      <c r="D48" s="66"/>
+      <c r="E48" s="55"/>
+      <c r="F48" s="65"/>
+      <c r="G48" s="70">
         <f>SUBTOTAL(9,G36:G47)</f>
         <v>176.5</v>
       </c>
-      <c r="H48" s="74">
+      <c r="H48" s="71">
         <f>SUBTOTAL(9,H36:H47)</f>
         <v>255</v>
       </c>
-      <c r="I48" s="75">
+      <c r="I48" s="72">
         <f>SUBTOTAL(9,I36:I47)</f>
         <v>1</v>
       </c>
-      <c r="J48" s="69"/>
-      <c r="K48" s="68"/>
-      <c r="L48" s="93">
+      <c r="J48" s="66"/>
+      <c r="K48" s="65"/>
+      <c r="L48" s="90">
         <f>SUBTOTAL(9,L36:L47)</f>
         <v>122014216.54151419</v>
       </c>
-      <c r="M48" s="70"/>
-      <c r="N48" s="93">
+      <c r="M48" s="67"/>
+      <c r="N48" s="90">
         <f>SUBTOTAL(9,N36:N47)</f>
         <v>7730432.1954625398</v>
       </c>
-      <c r="O48" s="62"/>
-      <c r="P48" s="60"/>
+      <c r="O48" s="59"/>
+      <c r="P48" s="57"/>
       <c r="Q48" s="6"/>
       <c r="R48" s="6"/>
       <c r="S48" s="6"/>
@@ -12342,18 +12379,18 @@
     <row r="49" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="6"/>
       <c r="B49" s="6"/>
-      <c r="C49" s="58"/>
+      <c r="C49" s="55"/>
       <c r="D49" s="6"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
-      <c r="G49" s="58"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
+      <c r="G49" s="55"/>
+      <c r="H49" s="55"/>
+      <c r="I49" s="55"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
-      <c r="L49" s="58"/>
+      <c r="L49" s="55"/>
       <c r="M49" s="6"/>
-      <c r="N49" s="58"/>
+      <c r="N49" s="55"/>
       <c r="O49" s="6"/>
       <c r="P49" s="6"/>
       <c r="Q49" s="6"/>
@@ -12426,22 +12463,22 @@
     <row r="52" spans="1:26" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="6"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="117" t="s">
-        <v>24</v>
-      </c>
-      <c r="D52" s="120"/>
-      <c r="E52" s="120"/>
-      <c r="F52" s="120"/>
-      <c r="G52" s="120"/>
-      <c r="H52" s="120"/>
-      <c r="I52" s="120"/>
-      <c r="J52" s="120"/>
-      <c r="K52" s="120"/>
-      <c r="L52" s="120"/>
-      <c r="M52" s="120"/>
-      <c r="N52" s="120"/>
-      <c r="O52" s="120"/>
-      <c r="P52" s="121"/>
+      <c r="C52" s="121" t="s">
+        <v>36</v>
+      </c>
+      <c r="D52" s="124"/>
+      <c r="E52" s="124"/>
+      <c r="F52" s="124"/>
+      <c r="G52" s="124"/>
+      <c r="H52" s="124"/>
+      <c r="I52" s="124"/>
+      <c r="J52" s="124"/>
+      <c r="K52" s="124"/>
+      <c r="L52" s="124"/>
+      <c r="M52" s="124"/>
+      <c r="N52" s="124"/>
+      <c r="O52" s="124"/>
+      <c r="P52" s="125"/>
       <c r="Q52" s="6"/>
       <c r="R52" s="6"/>
       <c r="S52" s="6"/>
@@ -12455,44 +12492,44 @@
     </row>
     <row r="53" spans="1:26" ht="18.75" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="6"/>
-      <c r="B53" s="52"/>
-      <c r="C53" s="124" t="s">
+      <c r="B53" s="51"/>
+      <c r="C53" s="114" t="s">
         <v>10</v>
       </c>
-      <c r="D53" s="122" t="s">
+      <c r="D53" s="112" t="s">
         <v>11</v>
       </c>
-      <c r="E53" s="122"/>
-      <c r="F53" s="122"/>
-      <c r="G53" s="124" t="s">
+      <c r="E53" s="112"/>
+      <c r="F53" s="112"/>
+      <c r="G53" s="114" t="s">
         <v>9</v>
       </c>
-      <c r="H53" s="122" t="s">
+      <c r="H53" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="I53" s="122" t="s">
+      <c r="I53" s="112" t="s">
         <v>7</v>
       </c>
-      <c r="J53" s="122" t="s">
+      <c r="J53" s="112" t="s">
         <v>6</v>
       </c>
-      <c r="K53" s="122" t="s">
+      <c r="K53" s="112" t="s">
         <v>8</v>
       </c>
-      <c r="L53" s="122" t="s">
+      <c r="L53" s="112" t="s">
         <v>15</v>
       </c>
-      <c r="M53" s="122" t="s">
+      <c r="M53" s="112" t="s">
         <v>18</v>
       </c>
-      <c r="N53" s="122" t="s">
+      <c r="N53" s="112" t="s">
         <v>1</v>
       </c>
-      <c r="O53" s="126" t="s">
+      <c r="O53" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="P53" s="126"/>
-      <c r="Q53" s="53"/>
+      <c r="P53" s="111"/>
+      <c r="Q53" s="52"/>
       <c r="R53" s="6"/>
       <c r="S53" s="6"/>
       <c r="T53" s="6"/>
@@ -12505,30 +12542,30 @@
     </row>
     <row r="54" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="6"/>
-      <c r="B54" s="52"/>
-      <c r="C54" s="125"/>
-      <c r="D54" s="54" t="s">
+      <c r="B54" s="51"/>
+      <c r="C54" s="116"/>
+      <c r="D54" s="134" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="28"/>
-      <c r="F54" s="54" t="s">
+      <c r="E54" s="135"/>
+      <c r="F54" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="G54" s="125"/>
-      <c r="H54" s="123"/>
-      <c r="I54" s="123"/>
-      <c r="J54" s="123"/>
-      <c r="K54" s="123"/>
-      <c r="L54" s="123"/>
-      <c r="M54" s="123"/>
-      <c r="N54" s="123"/>
-      <c r="O54" s="54" t="s">
+      <c r="G54" s="116"/>
+      <c r="H54" s="117"/>
+      <c r="I54" s="117"/>
+      <c r="J54" s="117"/>
+      <c r="K54" s="117"/>
+      <c r="L54" s="117"/>
+      <c r="M54" s="117"/>
+      <c r="N54" s="117"/>
+      <c r="O54" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="P54" s="54" t="s">
+      <c r="P54" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="Q54" s="53"/>
+      <c r="Q54" s="52"/>
       <c r="R54" s="6"/>
       <c r="S54" s="6"/>
       <c r="T54" s="6"/>
@@ -12541,50 +12578,50 @@
     </row>
     <row r="55" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="6"/>
-      <c r="B55" s="52"/>
-      <c r="C55" s="63">
+      <c r="B55" s="51"/>
+      <c r="C55" s="60">
         <v>1</v>
       </c>
-      <c r="D55" s="64">
+      <c r="D55" s="128">
         <v>1</v>
       </c>
-      <c r="E55" s="64" t="s">
+      <c r="E55" s="61" t="s">
         <v>4</v>
       </c>
-      <c r="F55" s="64">
+      <c r="F55" s="131">
         <v>31</v>
       </c>
-      <c r="G55" s="64">
+      <c r="G55" s="61">
         <f>(F55-D55)/2</f>
         <v>15</v>
       </c>
-      <c r="H55" s="64">
+      <c r="H55" s="61">
         <v>22</v>
       </c>
-      <c r="I55" s="65">
+      <c r="I55" s="62">
         <f t="shared" ref="I55:I66" si="17">H55/$H$30</f>
         <v>8.6274509803921567E-2</v>
       </c>
-      <c r="J55" s="64">
+      <c r="J55" s="61">
         <v>22</v>
       </c>
-      <c r="K55" s="66">
+      <c r="K55" s="63">
         <f>I55</f>
         <v>8.6274509803921567E-2</v>
       </c>
-      <c r="L55" s="92">
+      <c r="L55" s="89">
         <f>S2* 4.38</f>
         <v>39420000</v>
       </c>
-      <c r="M55" s="112">
+      <c r="M55" s="109">
         <f>(M18+M36)</f>
         <v>0.12</v>
       </c>
-      <c r="N55" s="94">
+      <c r="N55" s="91">
         <f>L55*M55</f>
         <v>4730400</v>
       </c>
-      <c r="O55" s="55"/>
+      <c r="O55" s="54"/>
       <c r="P55" s="17"/>
       <c r="Q55" s="6"/>
       <c r="R55" s="6"/>
@@ -12599,17 +12636,17 @@
     </row>
     <row r="56" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="6"/>
-      <c r="B56" s="52"/>
+      <c r="B56" s="51"/>
       <c r="C56" s="18">
         <v>2</v>
       </c>
-      <c r="D56" s="22">
+      <c r="D56" s="129">
         <v>1</v>
       </c>
       <c r="E56" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F56" s="22">
+      <c r="F56" s="132">
         <v>28</v>
       </c>
       <c r="G56" s="22">
@@ -12631,19 +12668,19 @@
         <f>I56+K55</f>
         <v>0.16470588235294117</v>
       </c>
-      <c r="L56" s="113">
+      <c r="L56" s="110">
         <f>L55-N55</f>
         <v>34689600</v>
       </c>
-      <c r="M56" s="110">
+      <c r="M56" s="107">
         <f t="shared" ref="M56:M66" si="20">(M19+M37)</f>
         <v>0.12</v>
       </c>
-      <c r="N56" s="95">
+      <c r="N56" s="92">
         <f t="shared" ref="N56:N66" si="21">L56*M56</f>
         <v>4162752</v>
       </c>
-      <c r="O56" s="76"/>
+      <c r="O56" s="73"/>
       <c r="P56" s="27"/>
       <c r="Q56" s="6"/>
       <c r="R56" s="6"/>
@@ -12658,17 +12695,17 @@
     </row>
     <row r="57" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="6"/>
-      <c r="B57" s="52"/>
+      <c r="B57" s="51"/>
       <c r="C57" s="18">
         <v>3</v>
       </c>
-      <c r="D57" s="22">
+      <c r="D57" s="129">
         <v>1</v>
       </c>
       <c r="E57" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F57" s="22">
+      <c r="F57" s="132">
         <v>31</v>
       </c>
       <c r="G57" s="22">
@@ -12690,27 +12727,27 @@
         <f t="shared" ref="K57:K66" si="22">I57+K56</f>
         <v>0.24313725490196078</v>
       </c>
-      <c r="L57" s="83">
+      <c r="L57" s="80">
         <f t="shared" ref="L57:L66" si="23">L56-N56</f>
         <v>30526848</v>
       </c>
-      <c r="M57" s="110">
+      <c r="M57" s="107">
         <f t="shared" si="20"/>
         <v>0.12</v>
       </c>
-      <c r="N57" s="89">
+      <c r="N57" s="86">
         <f t="shared" si="21"/>
         <v>3663221.76</v>
       </c>
-      <c r="O57" s="93">
+      <c r="O57" s="90">
         <f>AVERAGE(L55:L57)</f>
         <v>34878816</v>
       </c>
-      <c r="P57" s="93">
+      <c r="P57" s="90">
         <f>AVERAGE(N55:N57)</f>
         <v>4185457.92</v>
       </c>
-      <c r="Q57" s="53"/>
+      <c r="Q57" s="52"/>
       <c r="R57" s="6"/>
       <c r="S57" s="6"/>
       <c r="T57" s="6"/>
@@ -12723,17 +12760,17 @@
     </row>
     <row r="58" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6"/>
-      <c r="B58" s="52"/>
+      <c r="B58" s="51"/>
       <c r="C58" s="18">
         <v>4</v>
       </c>
-      <c r="D58" s="22">
+      <c r="D58" s="129">
         <v>1</v>
       </c>
       <c r="E58" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F58" s="22">
+      <c r="F58" s="132">
         <v>30</v>
       </c>
       <c r="G58" s="22">
@@ -12755,19 +12792,19 @@
         <f t="shared" si="22"/>
         <v>0.32549019607843138</v>
       </c>
-      <c r="L58" s="83">
+      <c r="L58" s="80">
         <f t="shared" si="23"/>
         <v>26863626.240000002</v>
       </c>
-      <c r="M58" s="110">
+      <c r="M58" s="107">
         <f t="shared" si="20"/>
         <v>0.14760000000000001</v>
       </c>
-      <c r="N58" s="95">
+      <c r="N58" s="92">
         <f t="shared" si="21"/>
         <v>3965071.2330240007</v>
       </c>
-      <c r="O58" s="55"/>
+      <c r="O58" s="54"/>
       <c r="P58" s="17"/>
       <c r="Q58" s="6"/>
       <c r="R58" s="6"/>
@@ -12782,17 +12819,17 @@
     </row>
     <row r="59" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="6"/>
-      <c r="B59" s="52"/>
+      <c r="B59" s="51"/>
       <c r="C59" s="18">
         <v>5</v>
       </c>
-      <c r="D59" s="22">
+      <c r="D59" s="129">
         <v>1</v>
       </c>
       <c r="E59" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F59" s="22">
+      <c r="F59" s="132">
         <v>31</v>
       </c>
       <c r="G59" s="22">
@@ -12814,19 +12851,19 @@
         <f t="shared" si="22"/>
         <v>0.41176470588235292</v>
       </c>
-      <c r="L59" s="83">
+      <c r="L59" s="80">
         <f t="shared" si="23"/>
         <v>22898555.006976001</v>
       </c>
-      <c r="M59" s="110">
+      <c r="M59" s="107">
         <f t="shared" si="20"/>
         <v>0.14760000000000001</v>
       </c>
-      <c r="N59" s="95">
+      <c r="N59" s="92">
         <f t="shared" si="21"/>
         <v>3379826.719029658</v>
       </c>
-      <c r="O59" s="76"/>
+      <c r="O59" s="73"/>
       <c r="P59" s="27"/>
       <c r="Q59" s="6"/>
       <c r="R59" s="6"/>
@@ -12841,17 +12878,17 @@
     </row>
     <row r="60" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6"/>
-      <c r="B60" s="52"/>
+      <c r="B60" s="51"/>
       <c r="C60" s="18">
         <v>6</v>
       </c>
-      <c r="D60" s="22">
+      <c r="D60" s="129">
         <v>1</v>
       </c>
       <c r="E60" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F60" s="22">
+      <c r="F60" s="132">
         <v>30</v>
       </c>
       <c r="G60" s="22">
@@ -12873,27 +12910,27 @@
         <f t="shared" si="22"/>
         <v>0.49019607843137253</v>
       </c>
-      <c r="L60" s="83">
+      <c r="L60" s="80">
         <f t="shared" si="23"/>
         <v>19518728.287946343</v>
       </c>
-      <c r="M60" s="110">
+      <c r="M60" s="107">
         <f t="shared" si="20"/>
         <v>0.12</v>
       </c>
-      <c r="N60" s="89">
+      <c r="N60" s="86">
         <f t="shared" si="21"/>
         <v>2342247.3945535612</v>
       </c>
-      <c r="O60" s="93">
+      <c r="O60" s="90">
         <f t="shared" ref="O60" si="24">AVERAGE(L58:L60)</f>
         <v>23093636.511640783</v>
       </c>
-      <c r="P60" s="93">
+      <c r="P60" s="90">
         <f>AVERAGE(N58:N60)</f>
         <v>3229048.4488690733</v>
       </c>
-      <c r="Q60" s="53"/>
+      <c r="Q60" s="52"/>
       <c r="R60" s="6"/>
       <c r="S60" s="6"/>
       <c r="T60" s="6"/>
@@ -12906,17 +12943,17 @@
     </row>
     <row r="61" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="6"/>
-      <c r="B61" s="52"/>
+      <c r="B61" s="51"/>
       <c r="C61" s="18">
         <v>7</v>
       </c>
-      <c r="D61" s="22">
+      <c r="D61" s="129">
         <v>1</v>
       </c>
       <c r="E61" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F61" s="22">
+      <c r="F61" s="132">
         <v>31</v>
       </c>
       <c r="G61" s="22">
@@ -12938,19 +12975,19 @@
         <f t="shared" si="22"/>
         <v>0.58039215686274503</v>
       </c>
-      <c r="L61" s="83">
+      <c r="L61" s="80">
         <f t="shared" si="23"/>
         <v>17176480.893392783</v>
       </c>
-      <c r="M61" s="110">
+      <c r="M61" s="107">
         <f t="shared" si="20"/>
         <v>0.12</v>
       </c>
-      <c r="N61" s="95">
+      <c r="N61" s="92">
         <f t="shared" si="21"/>
         <v>2061177.7072071338</v>
       </c>
-      <c r="O61" s="55"/>
+      <c r="O61" s="54"/>
       <c r="P61" s="17"/>
       <c r="Q61" s="6"/>
       <c r="R61" s="6"/>
@@ -12965,17 +13002,17 @@
     </row>
     <row r="62" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="6"/>
-      <c r="B62" s="52"/>
+      <c r="B62" s="51"/>
       <c r="C62" s="18">
         <v>8</v>
       </c>
-      <c r="D62" s="22">
+      <c r="D62" s="129">
         <v>1</v>
       </c>
       <c r="E62" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F62" s="22">
+      <c r="F62" s="132">
         <v>31</v>
       </c>
       <c r="G62" s="22">
@@ -12997,19 +13034,19 @@
         <f t="shared" si="22"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="L62" s="83">
+      <c r="L62" s="80">
         <f t="shared" si="23"/>
         <v>15115303.186185649</v>
       </c>
-      <c r="M62" s="110">
+      <c r="M62" s="107">
         <f t="shared" si="20"/>
         <v>0.12</v>
       </c>
-      <c r="N62" s="95">
+      <c r="N62" s="92">
         <f t="shared" si="21"/>
         <v>1813836.3823422778</v>
       </c>
-      <c r="O62" s="76"/>
+      <c r="O62" s="73"/>
       <c r="P62" s="27"/>
       <c r="Q62" s="6"/>
       <c r="R62" s="6"/>
@@ -13024,17 +13061,17 @@
     </row>
     <row r="63" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="6"/>
-      <c r="B63" s="52"/>
+      <c r="B63" s="51"/>
       <c r="C63" s="18">
         <v>9</v>
       </c>
-      <c r="D63" s="22">
+      <c r="D63" s="129">
         <v>1</v>
       </c>
       <c r="E63" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F63" s="22">
+      <c r="F63" s="132">
         <v>30</v>
       </c>
       <c r="G63" s="22">
@@ -13056,27 +13093,27 @@
         <f t="shared" si="22"/>
         <v>0.74901960784313726</v>
       </c>
-      <c r="L63" s="83">
+      <c r="L63" s="80">
         <f t="shared" si="23"/>
         <v>13301466.803843372</v>
       </c>
-      <c r="M63" s="110">
+      <c r="M63" s="107">
         <f t="shared" si="20"/>
         <v>0.12</v>
       </c>
-      <c r="N63" s="89">
+      <c r="N63" s="86">
         <f t="shared" si="21"/>
         <v>1596176.0164612045</v>
       </c>
-      <c r="O63" s="93">
+      <c r="O63" s="90">
         <f t="shared" ref="O63" si="25">AVERAGE(L61:L63)</f>
         <v>15197750.294473933</v>
       </c>
-      <c r="P63" s="93">
+      <c r="P63" s="90">
         <f>AVERAGE(N61:N63)</f>
         <v>1823730.0353368719</v>
       </c>
-      <c r="Q63" s="53"/>
+      <c r="Q63" s="52"/>
       <c r="R63" s="6"/>
       <c r="S63" s="6"/>
       <c r="T63" s="6"/>
@@ -13089,17 +13126,17 @@
     </row>
     <row r="64" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="6"/>
-      <c r="B64" s="52"/>
+      <c r="B64" s="51"/>
       <c r="C64" s="18">
         <v>10</v>
       </c>
-      <c r="D64" s="22">
+      <c r="D64" s="129">
         <v>1</v>
       </c>
       <c r="E64" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F64" s="22">
+      <c r="F64" s="132">
         <v>31</v>
       </c>
       <c r="G64" s="22">
@@ -13121,19 +13158,19 @@
         <f t="shared" si="22"/>
         <v>0.83921568627450982</v>
       </c>
-      <c r="L64" s="83">
+      <c r="L64" s="80">
         <f t="shared" si="23"/>
         <v>11705290.787382167</v>
       </c>
-      <c r="M64" s="110">
+      <c r="M64" s="107">
         <f t="shared" si="20"/>
         <v>0.12</v>
       </c>
-      <c r="N64" s="95">
+      <c r="N64" s="92">
         <f t="shared" si="21"/>
         <v>1404634.8944858599</v>
       </c>
-      <c r="O64" s="55"/>
+      <c r="O64" s="54"/>
       <c r="P64" s="17"/>
       <c r="Q64" s="6"/>
       <c r="R64" s="6"/>
@@ -13148,17 +13185,17 @@
     </row>
     <row r="65" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="6"/>
-      <c r="B65" s="52"/>
+      <c r="B65" s="51"/>
       <c r="C65" s="18">
         <v>11</v>
       </c>
-      <c r="D65" s="22">
+      <c r="D65" s="129">
         <v>1</v>
       </c>
       <c r="E65" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="F65" s="22">
+      <c r="F65" s="132">
         <v>30</v>
       </c>
       <c r="G65" s="22">
@@ -13180,19 +13217,19 @@
         <f t="shared" si="22"/>
         <v>0.91764705882352948</v>
       </c>
-      <c r="L65" s="83">
+      <c r="L65" s="80">
         <f t="shared" si="23"/>
         <v>10300655.892896308</v>
       </c>
-      <c r="M65" s="110">
+      <c r="M65" s="107">
         <f t="shared" si="20"/>
         <v>0.12</v>
       </c>
-      <c r="N65" s="95">
+      <c r="N65" s="92">
         <f t="shared" si="21"/>
         <v>1236078.7071475568</v>
       </c>
-      <c r="O65" s="76"/>
+      <c r="O65" s="73"/>
       <c r="P65" s="27"/>
       <c r="Q65" s="6"/>
       <c r="R65" s="6"/>
@@ -13207,17 +13244,17 @@
     </row>
     <row r="66" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6"/>
-      <c r="B66" s="52"/>
+      <c r="B66" s="51"/>
       <c r="C66" s="25">
         <v>12</v>
       </c>
-      <c r="D66" s="1">
+      <c r="D66" s="130">
         <v>1</v>
       </c>
       <c r="E66" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F66" s="1">
+      <c r="F66" s="133">
         <v>31</v>
       </c>
       <c r="G66" s="16">
@@ -13235,31 +13272,31 @@
         <f t="shared" si="19"/>
         <v>255</v>
       </c>
-      <c r="K66" s="67">
+      <c r="K66" s="64">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="L66" s="84">
+      <c r="L66" s="81">
         <f t="shared" si="23"/>
         <v>9064577.1857487503</v>
       </c>
-      <c r="M66" s="111">
+      <c r="M66" s="108">
         <f t="shared" si="20"/>
         <v>0.14760000000000001</v>
       </c>
-      <c r="N66" s="90">
+      <c r="N66" s="87">
         <f t="shared" si="21"/>
         <v>1337931.5926165157</v>
       </c>
-      <c r="O66" s="93">
+      <c r="O66" s="90">
         <f t="shared" ref="O66" si="26">AVERAGE(L64:L66)</f>
         <v>10356841.28867574</v>
       </c>
-      <c r="P66" s="93">
+      <c r="P66" s="90">
         <f>AVERAGE(N64:N66)</f>
         <v>1326215.0647499773</v>
       </c>
-      <c r="Q66" s="53"/>
+      <c r="Q66" s="52"/>
       <c r="R66" s="6"/>
       <c r="S66" s="6"/>
       <c r="T66" s="6"/>
@@ -13272,37 +13309,37 @@
     </row>
     <row r="67" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="6"/>
-      <c r="B67" s="52"/>
-      <c r="C67" s="72" t="s">
+      <c r="B67" s="51"/>
+      <c r="C67" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="D67" s="69"/>
-      <c r="E67" s="58"/>
-      <c r="F67" s="68"/>
-      <c r="G67" s="73">
+      <c r="D67" s="66"/>
+      <c r="E67" s="55"/>
+      <c r="F67" s="65"/>
+      <c r="G67" s="70">
         <f>SUBTOTAL(9,G55:G66)</f>
         <v>176.5</v>
       </c>
-      <c r="H67" s="74">
+      <c r="H67" s="71">
         <f>SUBTOTAL(9,H55:H66)</f>
         <v>255</v>
       </c>
-      <c r="I67" s="75">
+      <c r="I67" s="72">
         <f>SUBTOTAL(9,I55:I66)</f>
         <v>1</v>
       </c>
-      <c r="J67" s="69"/>
-      <c r="K67" s="68"/>
-      <c r="L67" s="93">
+      <c r="J67" s="66"/>
+      <c r="K67" s="65"/>
+      <c r="L67" s="90">
         <f>SUBTOTAL(9,L55:L66)</f>
         <v>250581132.28437138</v>
       </c>
-      <c r="M67" s="70"/>
-      <c r="N67" s="93">
+      <c r="M67" s="67"/>
+      <c r="N67" s="90">
         <f>SUBTOTAL(9,N55:N66)</f>
         <v>31693354.406867772</v>
       </c>
-      <c r="O67" s="55"/>
+      <c r="O67" s="54"/>
       <c r="P67" s="17"/>
       <c r="Q67" s="6"/>
       <c r="R67" s="6"/>
@@ -13318,18 +13355,18 @@
     <row r="68" spans="1:26" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6"/>
       <c r="B68" s="6"/>
-      <c r="C68" s="58"/>
+      <c r="C68" s="55"/>
       <c r="D68" s="6"/>
       <c r="E68" s="6"/>
       <c r="F68" s="6"/>
-      <c r="G68" s="58"/>
-      <c r="H68" s="58"/>
-      <c r="I68" s="58"/>
+      <c r="G68" s="55"/>
+      <c r="H68" s="55"/>
+      <c r="I68" s="55"/>
       <c r="J68" s="6"/>
       <c r="K68" s="6"/>
-      <c r="L68" s="58"/>
+      <c r="L68" s="55"/>
       <c r="M68" s="6"/>
-      <c r="N68" s="58"/>
+      <c r="N68" s="55"/>
       <c r="O68" s="6"/>
       <c r="P68" s="6"/>
       <c r="Q68" s="6"/>
@@ -19869,26 +19906,6 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="G34:G35"/>
-    <mergeCell ref="H34:H35"/>
-    <mergeCell ref="D34:F34"/>
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="K34:K35"/>
-    <mergeCell ref="L34:L35"/>
-    <mergeCell ref="M34:M35"/>
-    <mergeCell ref="N34:N35"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="I34:I35"/>
-    <mergeCell ref="J16:J17"/>
     <mergeCell ref="C15:P15"/>
     <mergeCell ref="C33:P33"/>
     <mergeCell ref="C52:P52"/>
@@ -19905,6 +19922,26 @@
     <mergeCell ref="L53:L54"/>
     <mergeCell ref="K53:K54"/>
     <mergeCell ref="J34:J35"/>
+    <mergeCell ref="K34:K35"/>
+    <mergeCell ref="L34:L35"/>
+    <mergeCell ref="M34:M35"/>
+    <mergeCell ref="N34:N35"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="I34:I35"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="C34:C35"/>
+    <mergeCell ref="G34:G35"/>
+    <mergeCell ref="H34:H35"/>
+    <mergeCell ref="D34:F34"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="K16:K17"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>